<commit_message>
ammw - documentation for backend
</commit_message>
<xml_diff>
--- a/00_Document/03_Testing/Backend/01_テスト仕様書/管理者＿スタッフアップデートAPI＿テスト仕様書.xlsx
+++ b/00_Document/03_Testing/Backend/01_テスト仕様書/管理者＿スタッフアップデートAPI＿テスト仕様書.xlsx
@@ -3,18 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6BB813-9EB7-45DD-A360-F2EB3F80FBE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0DA7D7-EA0D-4ABC-8DE9-F5D3B20F2336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="606" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="606" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="表紙" sheetId="5" r:id="rId1"/>
-    <sheet name="基本情報（従業員）" sheetId="15" r:id="rId2"/>
+    <sheet name="基本情報（管理者）" sheetId="15" r:id="rId2"/>
     <sheet name="エビデンス" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">エビデンス!#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'基本情報（従業員）'!$1:$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'基本情報（管理者）'!$1:$4</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>作成日</t>
     <rPh sb="0" eb="3">
@@ -254,9 +254,6 @@
     <t>異常</t>
   </si>
   <si>
-    <t>01_001_003</t>
-  </si>
-  <si>
     <t>リクエスト</t>
   </si>
   <si>
@@ -838,22 +835,10 @@
     </r>
   </si>
   <si>
-    <t>エイ</t>
-  </si>
-  <si>
-    <t>リクエストヘッダー</t>
-  </si>
-  <si>
-    <t>リスポンスヘッダー</t>
-  </si>
-  <si>
     <t>作成者</t>
   </si>
   <si>
     <t>Phyu</t>
-  </si>
-  <si>
-    <t>01_002_001</t>
   </si>
   <si>
     <t>スタッフ</t>
@@ -861,9 +846,6 @@
   <si>
     <t xml:space="preserve">１．Gender を選ぶことがないとき
 </t>
-  </si>
-  <si>
-    <t>01_002_002</t>
   </si>
   <si>
     <t xml:space="preserve">１．すべてのデータ入力
@@ -904,6 +886,15 @@
   </si>
   <si>
     <t>スタッフアップデート (002)</t>
+  </si>
+  <si>
+    <t>カイン</t>
+  </si>
+  <si>
+    <t>01_002_002_01</t>
+  </si>
+  <si>
+    <t>01_002_002_02</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1308,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1336,12 +1327,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1369,131 +1354,131 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1525,23 +1510,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>338018</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>158827</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>27247</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>538283</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>71639</xdr:rowOff>
+      <xdr:rowOff>18630</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{093308C8-E259-F218-712F-F01B328079C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54F49FB8-79AC-48AB-1289-2E69C4C4F88F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1550,20 +1535,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5910143" y="1559002"/>
-          <a:ext cx="5772390" cy="2713162"/>
+          <a:off x="438150" y="1627447"/>
+          <a:ext cx="6086475" cy="2591708"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1574,23 +1554,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>564241</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>129613</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>582386</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>220170</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>194382</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>75248</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>94833</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A801BD6B-CC3F-1DAA-1201-E8FD9D7A6220}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09B83492-6BDA-5914-BD0D-5C8E09599897}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1599,314 +1579,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5517241" y="5330263"/>
-          <a:ext cx="6466304" cy="2865119"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>354082</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>551</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>166428</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>50243</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{891DD254-BCCF-6B04-940A-2D8F663136D2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12736582" y="1600751"/>
-          <a:ext cx="5384471" cy="2650017"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>4336</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>149005</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>618163</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>164072</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97A0AD6E-039D-62FB-33A2-465FE2431875}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13005961" y="5149630"/>
-          <a:ext cx="7424202" cy="3415492"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>318170</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>102879</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>190708</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>166794</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{448F6C3F-9D91-755F-9983-906337A276F1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5890295" y="9504054"/>
-          <a:ext cx="6063788" cy="2864265"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>10402</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>67353</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>157099</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C048EAF4-B5E0-592D-7D89-AC0E070D35CC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5582527" y="13269003"/>
-          <a:ext cx="4675898" cy="1689946"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>535710</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>114364</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>496538</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>25447</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC615287-9D98-58F5-086D-3E82939D7384}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13537335" y="9515539"/>
-          <a:ext cx="4913828" cy="2911458"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>500891</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>131195</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>367721</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>82890</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB2DF66D-41AF-4055-BDBC-EF4DCEBD2FA5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13502516" y="13932920"/>
-          <a:ext cx="3581580" cy="1351870"/>
+          <a:off x="6773636" y="1466850"/>
+          <a:ext cx="6922362" cy="3028533"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2231,152 +1912,152 @@
   </cols>
   <sheetData>
     <row r="13" spans="9:37" ht="16.149999999999999" customHeight="1">
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="9"/>
-      <c r="AA13" s="9"/>
-      <c r="AB13" s="9"/>
-      <c r="AC13" s="9"/>
-      <c r="AD13" s="9"/>
-      <c r="AE13" s="9"/>
-      <c r="AF13" s="9"/>
-      <c r="AG13" s="9"/>
-      <c r="AH13" s="9"/>
-      <c r="AI13" s="9"/>
-      <c r="AJ13" s="9"/>
-      <c r="AK13" s="9"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="7"/>
+      <c r="AI13" s="7"/>
+      <c r="AJ13" s="7"/>
+      <c r="AK13" s="7"/>
     </row>
     <row r="14" spans="9:37" ht="16.149999999999999" customHeight="1">
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="9"/>
-      <c r="AA14" s="9"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="9"/>
-      <c r="AF14" s="9"/>
-      <c r="AG14" s="9"/>
-      <c r="AH14" s="9"/>
-      <c r="AI14" s="9"/>
-      <c r="AJ14" s="9"/>
-      <c r="AK14" s="9"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="7"/>
+      <c r="AJ14" s="7"/>
+      <c r="AK14" s="7"/>
     </row>
     <row r="17" spans="8:38" ht="16.149999999999999" customHeight="1">
-      <c r="H17" s="12"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="10" t="s">
+      <c r="H17" s="10"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="12" t="s">
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="10" t="s">
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="12" t="s">
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="Z17" s="13"/>
-      <c r="AA17" s="13"/>
-      <c r="AB17" s="13"/>
-      <c r="AC17" s="14"/>
-      <c r="AD17" s="10" t="s">
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="12"/>
+      <c r="AD17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="AE17" s="10"/>
-      <c r="AF17" s="10"/>
-      <c r="AG17" s="10"/>
-      <c r="AH17" s="12" t="s">
+      <c r="AE17" s="8"/>
+      <c r="AF17" s="8"/>
+      <c r="AG17" s="8"/>
+      <c r="AH17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="AI17" s="13"/>
-      <c r="AJ17" s="13"/>
-      <c r="AK17" s="13"/>
-      <c r="AL17" s="14"/>
+      <c r="AI17" s="11"/>
+      <c r="AJ17" s="11"/>
+      <c r="AK17" s="11"/>
+      <c r="AL17" s="12"/>
     </row>
     <row r="18" spans="8:38" ht="36" customHeight="1">
-      <c r="H18" s="15" t="s">
+      <c r="H18" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="11">
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="9">
         <v>44941</v>
       </c>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="16"/>
-      <c r="Z18" s="16"/>
-      <c r="AA18" s="16"/>
-      <c r="AB18" s="16"/>
-      <c r="AC18" s="16"/>
-      <c r="AD18" s="11"/>
-      <c r="AE18" s="11"/>
-      <c r="AF18" s="11"/>
-      <c r="AG18" s="11"/>
-      <c r="AH18" s="16"/>
-      <c r="AI18" s="16"/>
-      <c r="AJ18" s="16"/>
-      <c r="AK18" s="16"/>
-      <c r="AL18" s="16"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="14"/>
+      <c r="AA18" s="14"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="14"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="9"/>
+      <c r="AG18" s="9"/>
+      <c r="AH18" s="14"/>
+      <c r="AI18" s="14"/>
+      <c r="AJ18" s="14"/>
+      <c r="AK18" s="14"/>
+      <c r="AL18" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -2412,9 +2093,9 @@
   </sheetPr>
   <dimension ref="A1:BM21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T6" sqref="T6:AH6"/>
+      <selection pane="bottomLeft" activeCell="AI7" sqref="AI7:AW7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.149999999999999" customHeight="1"/>
@@ -2427,526 +2108,532 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="16.149999999999999" customHeight="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="43" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="46"/>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="47"/>
-      <c r="AU1" s="51" t="s">
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="24"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="24"/>
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="24"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="AV1" s="29"/>
-      <c r="AW1" s="30"/>
-      <c r="AX1" s="53">
+      <c r="AV1" s="30"/>
+      <c r="AW1" s="31"/>
+      <c r="AX1" s="35">
         <v>44941</v>
       </c>
-      <c r="AY1" s="54"/>
-      <c r="AZ1" s="54"/>
-      <c r="BA1" s="54"/>
-      <c r="BB1" s="54"/>
-      <c r="BC1" s="55"/>
-      <c r="BD1" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="BE1" s="29"/>
-      <c r="BF1" s="30"/>
-      <c r="BG1" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="BH1" s="22"/>
-      <c r="BI1" s="22"/>
-      <c r="BJ1" s="23"/>
+      <c r="AY1" s="36"/>
+      <c r="AZ1" s="36"/>
+      <c r="BA1" s="36"/>
+      <c r="BB1" s="36"/>
+      <c r="BC1" s="37"/>
+      <c r="BD1" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="BE1" s="30"/>
+      <c r="BF1" s="31"/>
+      <c r="BG1" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="BH1" s="48"/>
+      <c r="BI1" s="48"/>
+      <c r="BJ1" s="49"/>
     </row>
     <row r="2" spans="1:65" ht="16.149999999999999" customHeight="1" thickBot="1">
-      <c r="A2" s="40"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="49"/>
-      <c r="AD2" s="49"/>
-      <c r="AE2" s="49"/>
-      <c r="AF2" s="49"/>
-      <c r="AG2" s="49"/>
-      <c r="AH2" s="49"/>
-      <c r="AI2" s="49"/>
-      <c r="AJ2" s="49"/>
-      <c r="AK2" s="49"/>
-      <c r="AL2" s="49"/>
-      <c r="AM2" s="49"/>
-      <c r="AN2" s="49"/>
-      <c r="AO2" s="49"/>
-      <c r="AP2" s="49"/>
-      <c r="AQ2" s="49"/>
-      <c r="AR2" s="49"/>
-      <c r="AS2" s="49"/>
-      <c r="AT2" s="50"/>
-      <c r="AU2" s="52"/>
-      <c r="AV2" s="32"/>
-      <c r="AW2" s="33"/>
-      <c r="AX2" s="56"/>
-      <c r="AY2" s="57"/>
-      <c r="AZ2" s="57"/>
-      <c r="BA2" s="57"/>
-      <c r="BB2" s="57"/>
-      <c r="BC2" s="58"/>
-      <c r="BD2" s="31"/>
-      <c r="BE2" s="32"/>
-      <c r="BF2" s="33"/>
-      <c r="BG2" s="24"/>
-      <c r="BH2" s="25"/>
-      <c r="BI2" s="25"/>
-      <c r="BJ2" s="26"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
+      <c r="AI2" s="27"/>
+      <c r="AJ2" s="27"/>
+      <c r="AK2" s="27"/>
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="27"/>
+      <c r="AQ2" s="27"/>
+      <c r="AR2" s="27"/>
+      <c r="AS2" s="27"/>
+      <c r="AT2" s="28"/>
+      <c r="AU2" s="32"/>
+      <c r="AV2" s="33"/>
+      <c r="AW2" s="34"/>
+      <c r="AX2" s="38"/>
+      <c r="AY2" s="39"/>
+      <c r="AZ2" s="39"/>
+      <c r="BA2" s="39"/>
+      <c r="BB2" s="39"/>
+      <c r="BC2" s="40"/>
+      <c r="BD2" s="54"/>
+      <c r="BE2" s="33"/>
+      <c r="BF2" s="34"/>
+      <c r="BG2" s="50"/>
+      <c r="BH2" s="51"/>
+      <c r="BI2" s="51"/>
+      <c r="BJ2" s="52"/>
     </row>
     <row r="3" spans="1:65" ht="8.1" customHeight="1"/>
     <row r="4" spans="1:65" s="2" customFormat="1" ht="16.149999999999999" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="34" t="s">
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="27" t="s">
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="27"/>
-      <c r="AF4" s="27"/>
-      <c r="AG4" s="27"/>
-      <c r="AH4" s="27"/>
-      <c r="AI4" s="27" t="s">
+      <c r="U4" s="41"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="41"/>
+      <c r="AB4" s="41"/>
+      <c r="AC4" s="41"/>
+      <c r="AD4" s="41"/>
+      <c r="AE4" s="41"/>
+      <c r="AF4" s="41"/>
+      <c r="AG4" s="41"/>
+      <c r="AH4" s="41"/>
+      <c r="AI4" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="AJ4" s="27"/>
-      <c r="AK4" s="27"/>
-      <c r="AL4" s="27"/>
-      <c r="AM4" s="27"/>
-      <c r="AN4" s="27"/>
-      <c r="AO4" s="27"/>
-      <c r="AP4" s="27"/>
-      <c r="AQ4" s="27"/>
-      <c r="AR4" s="27"/>
-      <c r="AS4" s="27"/>
-      <c r="AT4" s="27"/>
-      <c r="AU4" s="27"/>
-      <c r="AV4" s="27"/>
-      <c r="AW4" s="27"/>
-      <c r="AX4" s="27" t="s">
+      <c r="AJ4" s="41"/>
+      <c r="AK4" s="41"/>
+      <c r="AL4" s="41"/>
+      <c r="AM4" s="41"/>
+      <c r="AN4" s="41"/>
+      <c r="AO4" s="41"/>
+      <c r="AP4" s="41"/>
+      <c r="AQ4" s="41"/>
+      <c r="AR4" s="41"/>
+      <c r="AS4" s="41"/>
+      <c r="AT4" s="41"/>
+      <c r="AU4" s="41"/>
+      <c r="AV4" s="41"/>
+      <c r="AW4" s="41"/>
+      <c r="AX4" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="AY4" s="27"/>
-      <c r="AZ4" s="27"/>
-      <c r="BA4" s="27" t="s">
+      <c r="AY4" s="41"/>
+      <c r="AZ4" s="41"/>
+      <c r="BA4" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="BB4" s="27"/>
-      <c r="BC4" s="27"/>
-      <c r="BD4" s="27" t="s">
+      <c r="BB4" s="41"/>
+      <c r="BC4" s="41"/>
+      <c r="BD4" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="BE4" s="27"/>
-      <c r="BF4" s="27" t="s">
+      <c r="BE4" s="41"/>
+      <c r="BF4" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="BG4" s="27"/>
-      <c r="BH4" s="27"/>
-      <c r="BI4" s="27" t="s">
+      <c r="BG4" s="41"/>
+      <c r="BH4" s="41"/>
+      <c r="BI4" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="BJ4" s="27"/>
+      <c r="BJ4" s="41"/>
     </row>
     <row r="5" spans="1:65" ht="72" customHeight="1">
-      <c r="A5" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19" t="s">
+      <c r="A5" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19" t="s">
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" s="55"/>
+      <c r="Q5" s="55"/>
+      <c r="R5" s="55"/>
+      <c r="S5" s="55"/>
+      <c r="T5" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="U5" s="55"/>
+      <c r="V5" s="55"/>
+      <c r="W5" s="55"/>
+      <c r="X5" s="55"/>
+      <c r="Y5" s="55"/>
+      <c r="Z5" s="55"/>
+      <c r="AA5" s="55"/>
+      <c r="AB5" s="55"/>
+      <c r="AC5" s="55"/>
+      <c r="AD5" s="55"/>
+      <c r="AE5" s="55"/>
+      <c r="AF5" s="55"/>
+      <c r="AG5" s="55"/>
+      <c r="AH5" s="55"/>
+      <c r="AI5" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="19"/>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="19"/>
-      <c r="Z5" s="19"/>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="19"/>
-      <c r="AE5" s="19"/>
-      <c r="AF5" s="19"/>
-      <c r="AG5" s="19"/>
-      <c r="AH5" s="19"/>
-      <c r="AI5" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ5" s="19"/>
-      <c r="AK5" s="19"/>
-      <c r="AL5" s="19"/>
-      <c r="AM5" s="19"/>
-      <c r="AN5" s="19"/>
-      <c r="AO5" s="19"/>
-      <c r="AP5" s="19"/>
-      <c r="AQ5" s="19"/>
-      <c r="AR5" s="19"/>
-      <c r="AS5" s="19"/>
-      <c r="AT5" s="19"/>
-      <c r="AU5" s="19"/>
-      <c r="AV5" s="19"/>
-      <c r="AW5" s="19"/>
-      <c r="AX5" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="AY5" s="20"/>
-      <c r="AZ5" s="20"/>
-      <c r="BA5" s="17">
-        <v>44938</v>
-      </c>
-      <c r="BB5" s="17"/>
-      <c r="BC5" s="17"/>
-      <c r="BD5" s="18" t="s">
+      <c r="AJ5" s="55"/>
+      <c r="AK5" s="55"/>
+      <c r="AL5" s="55"/>
+      <c r="AM5" s="55"/>
+      <c r="AN5" s="55"/>
+      <c r="AO5" s="55"/>
+      <c r="AP5" s="55"/>
+      <c r="AQ5" s="55"/>
+      <c r="AR5" s="55"/>
+      <c r="AS5" s="55"/>
+      <c r="AT5" s="55"/>
+      <c r="AU5" s="55"/>
+      <c r="AV5" s="55"/>
+      <c r="AW5" s="55"/>
+      <c r="AX5" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="AY5" s="56"/>
+      <c r="AZ5" s="56"/>
+      <c r="BA5" s="45">
+        <v>44941</v>
+      </c>
+      <c r="BB5" s="45"/>
+      <c r="BC5" s="45"/>
+      <c r="BD5" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="BE5" s="18"/>
-      <c r="BF5" s="18"/>
-      <c r="BG5" s="18"/>
-      <c r="BH5" s="18"/>
-      <c r="BI5" s="17"/>
-      <c r="BJ5" s="17"/>
+      <c r="BE5" s="46"/>
+      <c r="BF5" s="46"/>
+      <c r="BG5" s="46"/>
+      <c r="BH5" s="46"/>
+      <c r="BI5" s="45"/>
+      <c r="BJ5" s="45"/>
       <c r="BM5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:65" ht="72" customHeight="1">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" s="55"/>
+      <c r="Q6" s="55"/>
+      <c r="R6" s="55"/>
+      <c r="S6" s="55"/>
+      <c r="T6" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="U6" s="55"/>
+      <c r="V6" s="55"/>
+      <c r="W6" s="55"/>
+      <c r="X6" s="55"/>
+      <c r="Y6" s="55"/>
+      <c r="Z6" s="55"/>
+      <c r="AA6" s="55"/>
+      <c r="AB6" s="55"/>
+      <c r="AC6" s="55"/>
+      <c r="AD6" s="55"/>
+      <c r="AE6" s="55"/>
+      <c r="AF6" s="55"/>
+      <c r="AG6" s="55"/>
+      <c r="AH6" s="55"/>
+      <c r="AI6" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ6" s="55"/>
+      <c r="AK6" s="55"/>
+      <c r="AL6" s="55"/>
+      <c r="AM6" s="55"/>
+      <c r="AN6" s="55"/>
+      <c r="AO6" s="55"/>
+      <c r="AP6" s="55"/>
+      <c r="AQ6" s="55"/>
+      <c r="AR6" s="55"/>
+      <c r="AS6" s="55"/>
+      <c r="AT6" s="55"/>
+      <c r="AU6" s="55"/>
+      <c r="AV6" s="55"/>
+      <c r="AW6" s="55"/>
+      <c r="AX6" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="U6" s="19"/>
-      <c r="V6" s="19"/>
-      <c r="W6" s="19"/>
-      <c r="X6" s="19"/>
-      <c r="Y6" s="19"/>
-      <c r="Z6" s="19"/>
-      <c r="AA6" s="19"/>
-      <c r="AB6" s="19"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="19"/>
-      <c r="AE6" s="19"/>
-      <c r="AF6" s="19"/>
-      <c r="AG6" s="19"/>
-      <c r="AH6" s="19"/>
-      <c r="AI6" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ6" s="19"/>
-      <c r="AK6" s="19"/>
-      <c r="AL6" s="19"/>
-      <c r="AM6" s="19"/>
-      <c r="AN6" s="19"/>
-      <c r="AO6" s="19"/>
-      <c r="AP6" s="19"/>
-      <c r="AQ6" s="19"/>
-      <c r="AR6" s="19"/>
-      <c r="AS6" s="19"/>
-      <c r="AT6" s="19"/>
-      <c r="AU6" s="19"/>
-      <c r="AV6" s="19"/>
-      <c r="AW6" s="19"/>
-      <c r="AX6" s="20"/>
-      <c r="AY6" s="20"/>
-      <c r="AZ6" s="20"/>
-      <c r="BA6" s="17"/>
-      <c r="BB6" s="17"/>
-      <c r="BC6" s="17"/>
-      <c r="BD6" s="18"/>
-      <c r="BE6" s="18"/>
-      <c r="BF6" s="18"/>
-      <c r="BG6" s="18"/>
-      <c r="BH6" s="18"/>
-      <c r="BI6" s="17"/>
-      <c r="BJ6" s="17"/>
+      <c r="AY6" s="56"/>
+      <c r="AZ6" s="56"/>
+      <c r="BA6" s="45">
+        <v>44942</v>
+      </c>
+      <c r="BB6" s="45"/>
+      <c r="BC6" s="45"/>
+      <c r="BD6" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="BE6" s="46"/>
+      <c r="BF6" s="46"/>
+      <c r="BG6" s="46"/>
+      <c r="BH6" s="46"/>
+      <c r="BI6" s="45"/>
+      <c r="BJ6" s="45"/>
       <c r="BM6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:65" ht="75" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
-      <c r="V7" s="19"/>
-      <c r="W7" s="19"/>
-      <c r="X7" s="19"/>
-      <c r="Y7" s="19"/>
-      <c r="Z7" s="19"/>
-      <c r="AA7" s="19"/>
-      <c r="AB7" s="19"/>
-      <c r="AC7" s="19"/>
-      <c r="AD7" s="19"/>
-      <c r="AE7" s="19"/>
-      <c r="AF7" s="19"/>
-      <c r="AG7" s="19"/>
-      <c r="AH7" s="19"/>
-      <c r="AI7" s="19"/>
-      <c r="AJ7" s="19"/>
-      <c r="AK7" s="19"/>
-      <c r="AL7" s="19"/>
-      <c r="AM7" s="19"/>
-      <c r="AN7" s="19"/>
-      <c r="AO7" s="19"/>
-      <c r="AP7" s="19"/>
-      <c r="AQ7" s="19"/>
-      <c r="AR7" s="19"/>
-      <c r="AS7" s="19"/>
-      <c r="AT7" s="19"/>
-      <c r="AU7" s="19"/>
-      <c r="AV7" s="19"/>
-      <c r="AW7" s="19"/>
-      <c r="AX7" s="20"/>
-      <c r="AY7" s="20"/>
-      <c r="AZ7" s="20"/>
-      <c r="BA7" s="17"/>
-      <c r="BB7" s="17"/>
-      <c r="BC7" s="17"/>
-      <c r="BD7" s="18"/>
-      <c r="BE7" s="18"/>
-      <c r="BF7" s="18"/>
-      <c r="BG7" s="18"/>
-      <c r="BH7" s="18"/>
-      <c r="BI7" s="17"/>
-      <c r="BJ7" s="17"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="55"/>
+      <c r="Q7" s="55"/>
+      <c r="R7" s="55"/>
+      <c r="S7" s="55"/>
+      <c r="T7" s="55"/>
+      <c r="U7" s="55"/>
+      <c r="V7" s="55"/>
+      <c r="W7" s="55"/>
+      <c r="X7" s="55"/>
+      <c r="Y7" s="55"/>
+      <c r="Z7" s="55"/>
+      <c r="AA7" s="55"/>
+      <c r="AB7" s="55"/>
+      <c r="AC7" s="55"/>
+      <c r="AD7" s="55"/>
+      <c r="AE7" s="55"/>
+      <c r="AF7" s="55"/>
+      <c r="AG7" s="55"/>
+      <c r="AH7" s="55"/>
+      <c r="AI7" s="55"/>
+      <c r="AJ7" s="55"/>
+      <c r="AK7" s="55"/>
+      <c r="AL7" s="55"/>
+      <c r="AM7" s="55"/>
+      <c r="AN7" s="55"/>
+      <c r="AO7" s="55"/>
+      <c r="AP7" s="55"/>
+      <c r="AQ7" s="55"/>
+      <c r="AR7" s="55"/>
+      <c r="AS7" s="55"/>
+      <c r="AT7" s="55"/>
+      <c r="AU7" s="55"/>
+      <c r="AV7" s="55"/>
+      <c r="AW7" s="55"/>
+      <c r="AX7" s="56"/>
+      <c r="AY7" s="56"/>
+      <c r="AZ7" s="56"/>
+      <c r="BA7" s="45"/>
+      <c r="BB7" s="45"/>
+      <c r="BC7" s="45"/>
+      <c r="BD7" s="46"/>
+      <c r="BE7" s="46"/>
+      <c r="BF7" s="46"/>
+      <c r="BG7" s="46"/>
+      <c r="BH7" s="46"/>
+      <c r="BI7" s="45"/>
+      <c r="BJ7" s="45"/>
       <c r="BM7" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:65" ht="75" customHeight="1">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
-      <c r="V8" s="19"/>
-      <c r="W8" s="19"/>
-      <c r="X8" s="19"/>
-      <c r="Y8" s="19"/>
-      <c r="Z8" s="19"/>
-      <c r="AA8" s="19"/>
-      <c r="AB8" s="19"/>
-      <c r="AC8" s="19"/>
-      <c r="AD8" s="19"/>
-      <c r="AE8" s="19"/>
-      <c r="AF8" s="19"/>
-      <c r="AG8" s="19"/>
-      <c r="AH8" s="19"/>
-      <c r="AI8" s="19"/>
-      <c r="AJ8" s="19"/>
-      <c r="AK8" s="19"/>
-      <c r="AL8" s="19"/>
-      <c r="AM8" s="19"/>
-      <c r="AN8" s="19"/>
-      <c r="AO8" s="19"/>
-      <c r="AP8" s="19"/>
-      <c r="AQ8" s="19"/>
-      <c r="AR8" s="19"/>
-      <c r="AS8" s="19"/>
-      <c r="AT8" s="19"/>
-      <c r="AU8" s="19"/>
-      <c r="AV8" s="19"/>
-      <c r="AW8" s="19"/>
-      <c r="AX8" s="20"/>
-      <c r="AY8" s="20"/>
-      <c r="AZ8" s="20"/>
-      <c r="BA8" s="17"/>
-      <c r="BB8" s="17"/>
-      <c r="BC8" s="17"/>
-      <c r="BD8" s="18"/>
-      <c r="BE8" s="18"/>
-      <c r="BF8" s="18"/>
-      <c r="BG8" s="18"/>
-      <c r="BH8" s="18"/>
-      <c r="BI8" s="17"/>
-      <c r="BJ8" s="17"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="55"/>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="55"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="55"/>
+      <c r="U8" s="55"/>
+      <c r="V8" s="55"/>
+      <c r="W8" s="55"/>
+      <c r="X8" s="55"/>
+      <c r="Y8" s="55"/>
+      <c r="Z8" s="55"/>
+      <c r="AA8" s="55"/>
+      <c r="AB8" s="55"/>
+      <c r="AC8" s="55"/>
+      <c r="AD8" s="55"/>
+      <c r="AE8" s="55"/>
+      <c r="AF8" s="55"/>
+      <c r="AG8" s="55"/>
+      <c r="AH8" s="55"/>
+      <c r="AI8" s="55"/>
+      <c r="AJ8" s="55"/>
+      <c r="AK8" s="55"/>
+      <c r="AL8" s="55"/>
+      <c r="AM8" s="55"/>
+      <c r="AN8" s="55"/>
+      <c r="AO8" s="55"/>
+      <c r="AP8" s="55"/>
+      <c r="AQ8" s="55"/>
+      <c r="AR8" s="55"/>
+      <c r="AS8" s="55"/>
+      <c r="AT8" s="55"/>
+      <c r="AU8" s="55"/>
+      <c r="AV8" s="55"/>
+      <c r="AW8" s="55"/>
+      <c r="AX8" s="56"/>
+      <c r="AY8" s="56"/>
+      <c r="AZ8" s="56"/>
+      <c r="BA8" s="45"/>
+      <c r="BB8" s="45"/>
+      <c r="BC8" s="45"/>
+      <c r="BD8" s="46"/>
+      <c r="BE8" s="46"/>
+      <c r="BF8" s="46"/>
+      <c r="BG8" s="46"/>
+      <c r="BH8" s="46"/>
+      <c r="BI8" s="45"/>
+      <c r="BJ8" s="45"/>
       <c r="BM8" s="1" t="s">
         <v>24</v>
       </c>
@@ -3785,51 +3472,6 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A1:Q2"/>
-    <mergeCell ref="R1:W2"/>
-    <mergeCell ref="X1:AT2"/>
-    <mergeCell ref="AU1:AW2"/>
-    <mergeCell ref="AX1:BC2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="J4:S4"/>
-    <mergeCell ref="T4:AH4"/>
-    <mergeCell ref="AI4:AW4"/>
-    <mergeCell ref="BA5:BC5"/>
-    <mergeCell ref="BD5:BE5"/>
-    <mergeCell ref="BG1:BJ2"/>
-    <mergeCell ref="AX4:AZ4"/>
-    <mergeCell ref="BA4:BC4"/>
-    <mergeCell ref="BD4:BE4"/>
-    <mergeCell ref="BF4:BH4"/>
-    <mergeCell ref="BD1:BF2"/>
-    <mergeCell ref="BI4:BJ4"/>
-    <mergeCell ref="BF5:BH5"/>
-    <mergeCell ref="BI5:BJ5"/>
-    <mergeCell ref="AI5:AW5"/>
-    <mergeCell ref="AX5:AZ5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="O6:S6"/>
-    <mergeCell ref="T6:AH6"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="O5:S5"/>
-    <mergeCell ref="T5:AH5"/>
-    <mergeCell ref="BF6:BH6"/>
-    <mergeCell ref="BI6:BJ6"/>
-    <mergeCell ref="BF7:BH7"/>
-    <mergeCell ref="BI7:BJ7"/>
-    <mergeCell ref="AI6:AW6"/>
-    <mergeCell ref="AX6:AZ6"/>
-    <mergeCell ref="AI7:AW7"/>
-    <mergeCell ref="AX7:AZ7"/>
-    <mergeCell ref="BA7:BC7"/>
-    <mergeCell ref="BD7:BE7"/>
-    <mergeCell ref="BA6:BC6"/>
-    <mergeCell ref="BD6:BE6"/>
     <mergeCell ref="BI8:BJ8"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="E7:I7"/>
@@ -3846,6 +3488,51 @@
     <mergeCell ref="T8:AH8"/>
     <mergeCell ref="O7:S7"/>
     <mergeCell ref="T7:AH7"/>
+    <mergeCell ref="BF6:BH6"/>
+    <mergeCell ref="BI6:BJ6"/>
+    <mergeCell ref="BF7:BH7"/>
+    <mergeCell ref="BI7:BJ7"/>
+    <mergeCell ref="AI6:AW6"/>
+    <mergeCell ref="AX6:AZ6"/>
+    <mergeCell ref="AI7:AW7"/>
+    <mergeCell ref="AX7:AZ7"/>
+    <mergeCell ref="BA7:BC7"/>
+    <mergeCell ref="BD7:BE7"/>
+    <mergeCell ref="BA6:BC6"/>
+    <mergeCell ref="BD6:BE6"/>
+    <mergeCell ref="AI5:AW5"/>
+    <mergeCell ref="AX5:AZ5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="O6:S6"/>
+    <mergeCell ref="T6:AH6"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="O5:S5"/>
+    <mergeCell ref="T5:AH5"/>
+    <mergeCell ref="BA5:BC5"/>
+    <mergeCell ref="BD5:BE5"/>
+    <mergeCell ref="BG1:BJ2"/>
+    <mergeCell ref="AX4:AZ4"/>
+    <mergeCell ref="BA4:BC4"/>
+    <mergeCell ref="BD4:BE4"/>
+    <mergeCell ref="BF4:BH4"/>
+    <mergeCell ref="BD1:BF2"/>
+    <mergeCell ref="BI4:BJ4"/>
+    <mergeCell ref="BF5:BH5"/>
+    <mergeCell ref="BI5:BJ5"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:S4"/>
+    <mergeCell ref="T4:AH4"/>
+    <mergeCell ref="AI4:AW4"/>
+    <mergeCell ref="A1:Q2"/>
+    <mergeCell ref="R1:W2"/>
+    <mergeCell ref="X1:AT2"/>
+    <mergeCell ref="AU1:AW2"/>
+    <mergeCell ref="AX1:BC2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3859,324 +3546,260 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B3:BH79"/>
+  <dimension ref="A3:AY66"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B78" sqref="B78:D79"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.149999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="45" width="9.28515625" style="1" customWidth="1"/>
-    <col min="46" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="36" width="9.28515625" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:24" ht="16.149999999999999" customHeight="1">
-      <c r="B3" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-    </row>
-    <row r="4" spans="2:24" ht="16.149999999999999" customHeight="1">
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-    </row>
-    <row r="6" spans="2:24" ht="16.149999999999999" customHeight="1">
-      <c r="K6" s="60" t="s">
+    <row r="3" spans="2:18" ht="16.149999999999999" customHeight="1">
+      <c r="B3" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+    </row>
+    <row r="4" spans="2:18" ht="16.149999999999999" customHeight="1">
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+    </row>
+    <row r="6" spans="2:18" ht="16.149999999999999" customHeight="1">
+      <c r="B6" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="L6" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
-      <c r="U6" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="V6" s="60"/>
-      <c r="W6" s="60"/>
-      <c r="X6" s="60"/>
-    </row>
-    <row r="7" spans="2:24" ht="16.149999999999999" customHeight="1">
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
-      <c r="U7" s="60"/>
-      <c r="V7" s="60"/>
-      <c r="W7" s="60"/>
-      <c r="X7" s="60"/>
-    </row>
-    <row r="24" spans="11:25" ht="16.149999999999999" customHeight="1">
-      <c r="K24" s="59" t="s">
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="57"/>
+    </row>
+    <row r="7" spans="2:18" ht="16.149999999999999" customHeight="1">
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="57"/>
+      <c r="Q7" s="57"/>
+      <c r="R7" s="57"/>
+    </row>
+    <row r="24" spans="13:16" ht="16.149999999999999" customHeight="1">
+      <c r="M24" s="58"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="58"/>
+    </row>
+    <row r="25" spans="13:16" ht="16.149999999999999" customHeight="1">
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="58"/>
+    </row>
+    <row r="43" spans="1:51" ht="16.149999999999999" customHeight="1">
+      <c r="B43" s="59"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="59"/>
+    </row>
+    <row r="44" spans="1:51" ht="16.149999999999999" customHeight="1">
+      <c r="A44" s="6"/>
+      <c r="B44" s="59"/>
+      <c r="C44" s="59"/>
+      <c r="D44" s="59"/>
+      <c r="AD44" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L24" s="59"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="59"/>
-      <c r="O24" s="59"/>
-      <c r="P24" s="59"/>
-      <c r="Q24" s="59"/>
-      <c r="V24" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="W24" s="60"/>
-      <c r="X24" s="60"/>
-      <c r="Y24" s="60"/>
-    </row>
-    <row r="25" spans="11:25" ht="16.149999999999999" customHeight="1">
-      <c r="K25" s="59"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="59"/>
-      <c r="V25" s="60"/>
-      <c r="W25" s="60"/>
-      <c r="X25" s="60"/>
-      <c r="Y25" s="60"/>
-    </row>
-    <row r="44" spans="2:60" ht="16.149999999999999" customHeight="1">
-      <c r="B44" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="C44" s="61"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="7"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="AM44" s="5" t="s">
+    </row>
+    <row r="45" spans="1:51" ht="16.149999999999999" customHeight="1">
+      <c r="M45" s="58"/>
+      <c r="N45" s="58"/>
+      <c r="O45" s="58"/>
+      <c r="P45" s="58"/>
+      <c r="AD45" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="2:60" ht="16.149999999999999" customHeight="1">
-      <c r="B45" s="61"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="7"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="K45" s="60"/>
-      <c r="L45" s="60"/>
-      <c r="M45" s="60"/>
-      <c r="V45" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="W45" s="60"/>
-      <c r="X45" s="60"/>
-      <c r="Y45" s="60"/>
-      <c r="AM45" s="5" t="s">
+    <row r="46" spans="1:51" ht="16.149999999999999" customHeight="1">
+      <c r="M46" s="58"/>
+      <c r="N46" s="58"/>
+      <c r="O46" s="58"/>
+      <c r="P46" s="58"/>
+      <c r="AD46" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="46" spans="2:60" ht="16.149999999999999" customHeight="1">
-      <c r="J46" s="60"/>
-      <c r="K46" s="60"/>
-      <c r="L46" s="60"/>
-      <c r="M46" s="60"/>
-      <c r="V46" s="60"/>
-      <c r="W46" s="60"/>
-      <c r="X46" s="60"/>
-      <c r="Y46" s="60"/>
-      <c r="AM46" s="5" t="s">
+      <c r="AY46" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:51" ht="16.149999999999999" customHeight="1">
+      <c r="B47" s="58"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="58"/>
+      <c r="AD47" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="BH46" s="5" t="s">
+      <c r="AY47" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:51" ht="16.149999999999999" customHeight="1">
+      <c r="B48" s="58"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="58"/>
+      <c r="AD48" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AY48" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="2:60" ht="16.149999999999999" customHeight="1">
-      <c r="AM47" s="5" t="s">
+    <row r="49" spans="30:51" ht="16.149999999999999" customHeight="1">
+      <c r="AD49" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AY49" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="30:51" ht="16.149999999999999" customHeight="1">
+      <c r="AD50" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY50" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="30:51" ht="16.149999999999999" customHeight="1">
+      <c r="AD51" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AY51" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="30:51" ht="16.149999999999999" customHeight="1">
+      <c r="AD52" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AY52" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="BH47" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="2:60" ht="16.149999999999999" customHeight="1">
-      <c r="AM48" s="5" t="s">
+    </row>
+    <row r="53" spans="30:51" ht="16.149999999999999" customHeight="1">
+      <c r="AD53" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY53" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="BH48" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="AM49" s="5" t="s">
+    </row>
+    <row r="54" spans="30:51" ht="16.149999999999999" customHeight="1">
+      <c r="AD54" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AY54" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="BH49" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="AM50" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="BH50" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="AM51" s="5" t="s">
+    </row>
+    <row r="55" spans="30:51" ht="16.149999999999999" customHeight="1">
+      <c r="AY55" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="30:51" ht="16.149999999999999" customHeight="1">
+      <c r="AY56" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="30:51" ht="16.149999999999999" customHeight="1">
+      <c r="AY57" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="BH51" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="AM52" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="BH52" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="AM53" s="5" t="s">
+    </row>
+    <row r="58" spans="30:51" ht="16.149999999999999" customHeight="1">
+      <c r="AY58" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="30:51" ht="16.149999999999999" customHeight="1">
+      <c r="AY59" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60" spans="30:51" ht="16.149999999999999" customHeight="1">
+      <c r="AY60" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="61" spans="30:51" ht="16.149999999999999" customHeight="1">
+      <c r="AY61" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="BH53" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="AM54" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="BH54" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="55" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="BH55" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="56" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="BH56" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="57" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="BH57" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="58" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="BH58" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="59" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="BH59" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="60" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="BH60" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="61" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="BH61" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="63" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
-      <c r="H63" s="8"/>
-      <c r="I63" s="8"/>
-    </row>
-    <row r="64" spans="3:60" ht="16.149999999999999" customHeight="1">
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8"/>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
-    </row>
-    <row r="65" spans="2:26" ht="16.149999999999999" customHeight="1">
-      <c r="J65" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="K65" s="59"/>
-      <c r="L65" s="59"/>
-      <c r="M65" s="59"/>
-      <c r="N65" s="59"/>
-      <c r="O65" s="59"/>
-      <c r="P65" s="59"/>
-      <c r="W65" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="X65" s="60"/>
-      <c r="Y65" s="60"/>
-      <c r="Z65" s="60"/>
-    </row>
-    <row r="66" spans="2:26" ht="16.149999999999999" customHeight="1">
-      <c r="J66" s="59"/>
-      <c r="K66" s="59"/>
-      <c r="L66" s="59"/>
-      <c r="M66" s="59"/>
-      <c r="N66" s="59"/>
-      <c r="O66" s="59"/>
-      <c r="P66" s="59"/>
-      <c r="W66" s="60"/>
-      <c r="X66" s="60"/>
-      <c r="Y66" s="60"/>
-      <c r="Z66" s="60"/>
-    </row>
-    <row r="78" spans="2:26" ht="16.149999999999999" customHeight="1">
-      <c r="B78" s="61" t="s">
-        <v>25</v>
-      </c>
-      <c r="C78" s="61"/>
-      <c r="D78" s="61"/>
-    </row>
-    <row r="79" spans="2:26" ht="16.149999999999999" customHeight="1">
-      <c r="B79" s="61"/>
-      <c r="C79" s="61"/>
-      <c r="D79" s="61"/>
+    </row>
+    <row r="65" spans="1:17" ht="16.149999999999999" customHeight="1">
+      <c r="A65" s="57"/>
+      <c r="B65" s="57"/>
+      <c r="C65" s="57"/>
+      <c r="D65" s="57"/>
+      <c r="E65" s="57"/>
+      <c r="F65" s="57"/>
+      <c r="G65" s="57"/>
+      <c r="N65" s="58"/>
+      <c r="O65" s="58"/>
+      <c r="P65" s="58"/>
+      <c r="Q65" s="58"/>
+    </row>
+    <row r="66" spans="1:17" ht="16.149999999999999" customHeight="1">
+      <c r="A66" s="57"/>
+      <c r="B66" s="57"/>
+      <c r="C66" s="57"/>
+      <c r="D66" s="57"/>
+      <c r="E66" s="57"/>
+      <c r="F66" s="57"/>
+      <c r="G66" s="57"/>
+      <c r="N66" s="58"/>
+      <c r="O66" s="58"/>
+      <c r="P66" s="58"/>
+      <c r="Q66" s="58"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="J65:P66"/>
-    <mergeCell ref="W65:Z66"/>
-    <mergeCell ref="B78:D79"/>
-    <mergeCell ref="K24:Q25"/>
+  <mergeCells count="9">
+    <mergeCell ref="A65:G66"/>
+    <mergeCell ref="N65:Q66"/>
+    <mergeCell ref="L6:R7"/>
     <mergeCell ref="B3:H4"/>
-    <mergeCell ref="K6:N7"/>
-    <mergeCell ref="U6:X7"/>
-    <mergeCell ref="V24:Y25"/>
-    <mergeCell ref="B44:D45"/>
-    <mergeCell ref="J45:M46"/>
-    <mergeCell ref="V45:Y46"/>
+    <mergeCell ref="B6:E7"/>
+    <mergeCell ref="M24:P25"/>
+    <mergeCell ref="B43:D44"/>
+    <mergeCell ref="B47:E48"/>
+    <mergeCell ref="M45:P46"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>